<commit_message>
1/5 scale 2 box installation
</commit_message>
<xml_diff>
--- a/Config/Calibrations/CraneBayTwoBox/Calibration06142011.xlsx
+++ b/Config/Calibrations/CraneBayTwoBox/Calibration06142011.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="19035" windowHeight="12270" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="19035" windowHeight="12270" firstSheet="7" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="calibration_external_LVDT" sheetId="12" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Rough Calibration 2" sheetId="8" r:id="rId10"/>
     <sheet name="Comparison" sheetId="9" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -482,7 +482,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -538,11 +537,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="75419584"/>
-        <c:axId val="75420160"/>
+        <c:axId val="46835968"/>
+        <c:axId val="46836544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="75419584"/>
+        <c:axId val="46835968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -552,12 +551,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75420160"/>
+        <c:crossAx val="46836544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="75420160"/>
+        <c:axId val="46836544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -568,14 +567,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75419584"/>
+        <c:crossAx val="46835968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -620,7 +618,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -805,11 +802,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="145015360"/>
-        <c:axId val="145015936"/>
+        <c:axId val="89619200"/>
+        <c:axId val="89619776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="145015360"/>
+        <c:axId val="89619200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -831,19 +828,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145015936"/>
+        <c:crossAx val="89619776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="145015936"/>
+        <c:axId val="89619776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -866,14 +862,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145015360"/>
+        <c:crossAx val="89619200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -925,7 +920,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1115,11 +1109,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="145017664"/>
-        <c:axId val="145018240"/>
+        <c:axId val="90080384"/>
+        <c:axId val="90080960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="145017664"/>
+        <c:axId val="90080384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1146,19 +1140,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145018240"/>
+        <c:crossAx val="90080960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="145018240"/>
+        <c:axId val="90080960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1186,14 +1179,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145017664"/>
+        <c:crossAx val="90080384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1240,7 +1232,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1425,11 +1416,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="145019968"/>
-        <c:axId val="145020544"/>
+        <c:axId val="90082688"/>
+        <c:axId val="90083264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="145019968"/>
+        <c:axId val="90082688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1451,19 +1442,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145020544"/>
+        <c:crossAx val="90083264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="145020544"/>
+        <c:axId val="90083264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1486,14 +1476,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145019968"/>
+        <c:crossAx val="90082688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1540,7 +1529,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1725,11 +1713,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="145022272"/>
-        <c:axId val="148373504"/>
+        <c:axId val="90084992"/>
+        <c:axId val="90085568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="145022272"/>
+        <c:axId val="90084992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1751,19 +1739,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148373504"/>
+        <c:crossAx val="90085568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="148373504"/>
+        <c:axId val="90085568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1786,14 +1773,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145022272"/>
+        <c:crossAx val="90084992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1993,11 +1979,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="148376384"/>
-        <c:axId val="148376960"/>
+        <c:axId val="91858048"/>
+        <c:axId val="91858624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="148376384"/>
+        <c:axId val="91858048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2030,12 +2016,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148376960"/>
+        <c:crossAx val="91858624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="148376960"/>
+        <c:axId val="91858624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2069,7 +2055,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148376384"/>
+        <c:crossAx val="91858048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2264,11 +2250,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="148377536"/>
-        <c:axId val="148378112"/>
+        <c:axId val="91859200"/>
+        <c:axId val="91859776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="148377536"/>
+        <c:axId val="91859200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2296,12 +2282,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148378112"/>
+        <c:crossAx val="91859776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="148378112"/>
+        <c:axId val="91859776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2330,7 +2316,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148377536"/>
+        <c:crossAx val="91859200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2382,7 +2368,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2572,11 +2557,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="148379840"/>
-        <c:axId val="148380416"/>
+        <c:axId val="91861504"/>
+        <c:axId val="91862080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="148379840"/>
+        <c:axId val="91861504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2603,19 +2588,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148380416"/>
+        <c:crossAx val="91862080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="148380416"/>
+        <c:axId val="91862080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2643,14 +2627,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148379840"/>
+        <c:crossAx val="91861504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2697,7 +2680,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2839,11 +2821,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="148578880"/>
-        <c:axId val="148579456"/>
+        <c:axId val="91863808"/>
+        <c:axId val="91864384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="148578880"/>
+        <c:axId val="91863808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2870,19 +2852,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148579456"/>
+        <c:crossAx val="91864384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="148579456"/>
+        <c:axId val="91864384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2910,14 +2891,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148578880"/>
+        <c:crossAx val="91863808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2964,7 +2944,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3101,11 +3080,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="148581184"/>
-        <c:axId val="148581760"/>
+        <c:axId val="49398912"/>
+        <c:axId val="49399488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="148581184"/>
+        <c:axId val="49398912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3127,19 +3106,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148581760"/>
+        <c:crossAx val="49399488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="148581760"/>
+        <c:axId val="49399488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3162,14 +3140,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148581184"/>
+        <c:crossAx val="49398912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3221,7 +3198,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3363,11 +3339,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="148583488"/>
-        <c:axId val="148584064"/>
+        <c:axId val="49401216"/>
+        <c:axId val="49401792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="148583488"/>
+        <c:axId val="49401216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3394,19 +3370,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148584064"/>
+        <c:crossAx val="49401792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="148584064"/>
+        <c:axId val="49401792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3434,14 +3409,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148583488"/>
+        <c:crossAx val="49401216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3491,7 +3465,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -3559,11 +3532,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="75421888"/>
-        <c:axId val="75422464"/>
+        <c:axId val="46838272"/>
+        <c:axId val="46838848"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="75421888"/>
+        <c:axId val="46838272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3573,12 +3546,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75422464"/>
+        <c:crossAx val="46838848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="75422464"/>
+        <c:axId val="46838848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3589,14 +3562,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75421888"/>
+        <c:crossAx val="46838272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3641,7 +3613,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3778,11 +3749,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="148585792"/>
-        <c:axId val="149110784"/>
+        <c:axId val="49403520"/>
+        <c:axId val="49404096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="148585792"/>
+        <c:axId val="49403520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3804,19 +3775,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149110784"/>
+        <c:crossAx val="49404096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="149110784"/>
+        <c:axId val="49404096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3839,14 +3809,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148585792"/>
+        <c:crossAx val="49403520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3898,7 +3867,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4088,11 +4056,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="149112512"/>
-        <c:axId val="149113088"/>
+        <c:axId val="95223808"/>
+        <c:axId val="95224384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="149112512"/>
+        <c:axId val="95223808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4119,19 +4087,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149113088"/>
+        <c:crossAx val="95224384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="149113088"/>
+        <c:axId val="95224384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4159,14 +4126,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149112512"/>
+        <c:crossAx val="95223808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4213,7 +4179,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4398,11 +4363,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="149114816"/>
-        <c:axId val="149115392"/>
+        <c:axId val="95226112"/>
+        <c:axId val="95226688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="149114816"/>
+        <c:axId val="95226112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4424,19 +4389,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149115392"/>
+        <c:crossAx val="95226688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="149115392"/>
+        <c:axId val="95226688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4459,14 +4423,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149114816"/>
+        <c:crossAx val="95226112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4518,7 +4481,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4708,11 +4670,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="149117120"/>
-        <c:axId val="149117696"/>
+        <c:axId val="95228416"/>
+        <c:axId val="95228992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="149117120"/>
+        <c:axId val="95228416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4739,19 +4701,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149117696"/>
+        <c:crossAx val="95228992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="149117696"/>
+        <c:axId val="95228992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4779,14 +4740,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149117120"/>
+        <c:crossAx val="95228416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4833,7 +4793,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5018,11 +4977,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="149176896"/>
-        <c:axId val="149177472"/>
+        <c:axId val="95230720"/>
+        <c:axId val="95231296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="149176896"/>
+        <c:axId val="95230720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5044,19 +5003,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149177472"/>
+        <c:crossAx val="95231296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="149177472"/>
+        <c:axId val="95231296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5079,14 +5037,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149176896"/>
+        <c:crossAx val="95230720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5138,7 +5095,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5328,11 +5284,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="149179200"/>
-        <c:axId val="149179776"/>
+        <c:axId val="96814208"/>
+        <c:axId val="96814784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="149179200"/>
+        <c:axId val="96814208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5359,19 +5315,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149179776"/>
+        <c:crossAx val="96814784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="149179776"/>
+        <c:axId val="96814784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5399,14 +5354,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149179200"/>
+        <c:crossAx val="96814208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5453,7 +5407,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5638,11 +5591,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="149181504"/>
-        <c:axId val="149182080"/>
+        <c:axId val="96816512"/>
+        <c:axId val="96817088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="149181504"/>
+        <c:axId val="96816512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5664,19 +5617,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149182080"/>
+        <c:crossAx val="96817088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="149182080"/>
+        <c:axId val="96817088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5699,14 +5651,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149181504"/>
+        <c:crossAx val="96816512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5948,11 +5899,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="149183808"/>
-        <c:axId val="150052864"/>
+        <c:axId val="96818816"/>
+        <c:axId val="96819392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="149183808"/>
+        <c:axId val="96818816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5986,12 +5937,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150052864"/>
+        <c:crossAx val="96819392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="150052864"/>
+        <c:axId val="96819392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6026,7 +5977,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149183808"/>
+        <c:crossAx val="96818816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6258,11 +6209,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="150054592"/>
-        <c:axId val="150055168"/>
+        <c:axId val="132734976"/>
+        <c:axId val="132735552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="150054592"/>
+        <c:axId val="132734976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6291,12 +6242,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150055168"/>
+        <c:crossAx val="132735552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="150055168"/>
+        <c:axId val="132735552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6326,7 +6277,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150054592"/>
+        <c:crossAx val="132734976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6503,11 +6454,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="150056896"/>
-        <c:axId val="150057472"/>
+        <c:axId val="132737280"/>
+        <c:axId val="132737856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="150056896"/>
+        <c:axId val="132737280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6517,12 +6468,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150057472"/>
+        <c:crossAx val="132737856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="150057472"/>
+        <c:axId val="132737856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6533,7 +6484,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150056896"/>
+        <c:crossAx val="132737280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6580,7 +6531,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -6607,7 +6557,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="#,##0.00000000" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -6722,11 +6671,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="109068864"/>
-        <c:axId val="109069440"/>
+        <c:axId val="46840576"/>
+        <c:axId val="46841152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="109068864"/>
+        <c:axId val="46840576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6753,19 +6702,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109069440"/>
+        <c:crossAx val="46841152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="109069440"/>
+        <c:axId val="46841152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6793,14 +6741,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109068864"/>
+        <c:crossAx val="46840576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6977,11 +6924,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="150059200"/>
-        <c:axId val="150059776"/>
+        <c:axId val="132739584"/>
+        <c:axId val="132740160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="150059200"/>
+        <c:axId val="132739584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6991,12 +6938,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150059776"/>
+        <c:crossAx val="132740160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="150059776"/>
+        <c:axId val="132740160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7007,7 +6954,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150059200"/>
+        <c:crossAx val="132739584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7062,7 +7009,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -7184,11 +7130,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="145793600"/>
-        <c:axId val="145794176"/>
+        <c:axId val="132741888"/>
+        <c:axId val="132742464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="145793600"/>
+        <c:axId val="132741888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7198,12 +7144,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145794176"/>
+        <c:crossAx val="132742464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="145794176"/>
+        <c:axId val="132742464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7214,7 +7160,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145793600"/>
+        <c:crossAx val="132741888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7269,7 +7215,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -7391,11 +7336,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="145795904"/>
-        <c:axId val="145796480"/>
+        <c:axId val="132949120"/>
+        <c:axId val="132949696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="145795904"/>
+        <c:axId val="132949120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7405,12 +7350,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145796480"/>
+        <c:crossAx val="132949696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="145796480"/>
+        <c:axId val="132949696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7421,7 +7366,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145795904"/>
+        <c:crossAx val="132949120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7476,7 +7421,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -7598,11 +7542,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="145798208"/>
-        <c:axId val="145798784"/>
+        <c:axId val="132951424"/>
+        <c:axId val="132952000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="145798208"/>
+        <c:axId val="132951424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7612,12 +7556,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145798784"/>
+        <c:crossAx val="132952000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="145798784"/>
+        <c:axId val="132952000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7628,7 +7572,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145798208"/>
+        <c:crossAx val="132951424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7683,7 +7627,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -7805,11 +7748,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="145867328"/>
-        <c:axId val="145867904"/>
+        <c:axId val="132954880"/>
+        <c:axId val="132955456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="145867328"/>
+        <c:axId val="132954880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7819,12 +7762,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145867904"/>
+        <c:crossAx val="132955456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="145867904"/>
+        <c:axId val="132955456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7835,7 +7778,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145867328"/>
+        <c:crossAx val="132954880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7882,7 +7825,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -8019,11 +7961,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="109071168"/>
-        <c:axId val="109071744"/>
+        <c:axId val="49751168"/>
+        <c:axId val="49751744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="109071168"/>
+        <c:axId val="49751168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8045,19 +7987,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109071744"/>
+        <c:crossAx val="49751744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="109071744"/>
+        <c:axId val="49751744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8080,14 +8021,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109071168"/>
+        <c:crossAx val="49751168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8134,7 +8074,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -8161,7 +8100,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="#,##0.00000000" sourceLinked="0"/>
               <c:txPr>
                 <a:bodyPr/>
@@ -8288,11 +8226,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="109073472"/>
-        <c:axId val="109074048"/>
+        <c:axId val="49753472"/>
+        <c:axId val="49754048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="109073472"/>
+        <c:axId val="49753472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8319,19 +8257,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109074048"/>
+        <c:crossAx val="49754048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="109074048"/>
+        <c:axId val="49754048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8359,14 +8296,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109073472"/>
+        <c:crossAx val="49753472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8413,7 +8349,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -8550,11 +8485,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="109075776"/>
-        <c:axId val="110338048"/>
+        <c:axId val="49755776"/>
+        <c:axId val="49756352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="109075776"/>
+        <c:axId val="49755776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8576,19 +8511,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110338048"/>
+        <c:crossAx val="49756352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="110338048"/>
+        <c:axId val="49756352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8611,14 +8545,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109075776"/>
+        <c:crossAx val="49755776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8670,7 +8603,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -8860,11 +8792,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="110339776"/>
-        <c:axId val="110340352"/>
+        <c:axId val="89612288"/>
+        <c:axId val="89612864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="110339776"/>
+        <c:axId val="89612288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8891,19 +8823,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110340352"/>
+        <c:crossAx val="89612864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="110340352"/>
+        <c:axId val="89612864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8931,14 +8862,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110339776"/>
+        <c:crossAx val="89612288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8985,7 +8915,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -9170,11 +9099,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="110342080"/>
-        <c:axId val="110342656"/>
+        <c:axId val="89614592"/>
+        <c:axId val="89615168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="110342080"/>
+        <c:axId val="89614592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9196,19 +9125,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110342656"/>
+        <c:crossAx val="89615168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="110342656"/>
+        <c:axId val="89615168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9231,14 +9159,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110342080"/>
+        <c:crossAx val="89614592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9290,7 +9217,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -9480,11 +9406,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="110344384"/>
-        <c:axId val="110344960"/>
+        <c:axId val="89616896"/>
+        <c:axId val="89617472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="110344384"/>
+        <c:axId val="89616896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9511,19 +9437,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110344960"/>
+        <c:crossAx val="89617472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="110344960"/>
+        <c:axId val="89617472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9551,14 +9476,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110344384"/>
+        <c:crossAx val="89616896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12198,7 +12122,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D3:S56"/>
   <sheetViews>
-    <sheetView topLeftCell="D10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
       <selection activeCell="U28" sqref="U28"/>
     </sheetView>
   </sheetViews>
@@ -14414,7 +14338,7 @@
         <v>3.4548999999999999</v>
       </c>
       <c r="H37" s="3">
-        <f t="shared" ref="H37:H52" si="4">G37*$H$6</f>
+        <f t="shared" ref="H37:H48" si="4">G37*$H$6</f>
         <v>2.0712125499999998</v>
       </c>
       <c r="I37" s="3">
@@ -16579,7 +16503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
+    <sheetView topLeftCell="A166" workbookViewId="0">
       <selection activeCell="C166" sqref="C166"/>
     </sheetView>
   </sheetViews>

</xml_diff>